<commit_message>
integrate code for date top issue and main page more than 1 table
</commit_message>
<xml_diff>
--- a/LOGS/a5f6da06-f864-4636-80e8-db4a1edb1e66/main_page_service_output/notes_standard_cropped_df.xlsx
+++ b/LOGS/a5f6da06-f864-4636-80e8-db4a1edb1e66/main_page_service_output/notes_standard_cropped_df.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="44">
   <si>
     <t>line_item_0</t>
   </si>
@@ -35,6 +35,30 @@
     <t>header_col_0</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Finished goods</t>
+  </si>
+  <si>
+    <t>Goods in transit</t>
+  </si>
+  <si>
+    <t>Provision for inventory obsolescence</t>
+  </si>
+  <si>
+    <t>10 Inventories</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>header_col_1</t>
+  </si>
+  <si>
     <t>Trade payables</t>
   </si>
   <si>
@@ -50,15 +74,51 @@
     <t>$'000</t>
   </si>
   <si>
-    <t>header_col_1</t>
+    <t>Opening balance</t>
+  </si>
+  <si>
+    <t>Additions</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Closing balance</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Non-current</t>
+  </si>
+  <si>
+    <t>Interest on lease liabilities</t>
+  </si>
+  <si>
+    <t>Depreciation of right-of use assets</t>
+  </si>
+  <si>
+    <t>Total cash outflow for leases</t>
+  </si>
+  <si>
+    <t>13 Lease liabilities</t>
+  </si>
+  <si>
+    <t>Amounts recognised in profit or loss</t>
+  </si>
+  <si>
+    <t>Amounts recognised in the statement of cash flows</t>
+  </si>
+  <si>
+    <t>Liability for annual leave and other current employee benefits</t>
+  </si>
+  <si>
+    <t>Liability for long-service leave</t>
   </si>
   <si>
     <t>header_col_2</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>at 1 January</t>
   </si>
   <si>
@@ -69,12 +129,6 @@
   </si>
   <si>
     <t>Shares</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>2021</t>
   </si>
   <si>
     <t>A class ordinary shares</t>
@@ -456,12 +510,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>21156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>13236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>-73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>34319</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>14472</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>13324</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>-161</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>27635</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -480,13 +682,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,87 +701,141 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1564</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>19828</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>15277</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="C5">
         <v>36669</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>3752</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>19220</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>12092</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="C9">
         <v>35064</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -589,24 +845,490 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>11043</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>888</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>-4452</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>7638</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>3652</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>3986</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>159</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>2649</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>4293</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>1289</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>11685</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>-2009</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>11.043</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
+        <v>4090</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>6953</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>1.517</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>1931</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>1.139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1139</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>787</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>787</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>1218</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>1218</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>720</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>720</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>2021</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -633,30 +1355,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>8160000</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>2022</v>
@@ -664,19 +1386,19 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>8160000</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>2022</v>
@@ -687,13 +1409,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G4">
         <v>2022</v>
@@ -704,13 +1426,13 @@
         <v>2022</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G5">
         <v>2022</v>
@@ -721,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G6">
         <v>2022</v>
@@ -735,19 +1457,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>21840000</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G7">
         <v>2022</v>
@@ -755,19 +1477,19 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>21840000</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G8">
         <v>2022</v>
@@ -775,19 +1497,19 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>8.16</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>2021</v>
@@ -795,19 +1517,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>8160000</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>2021</v>
@@ -818,13 +1540,13 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <v>2021</v>
@@ -835,13 +1557,13 @@
         <v>2021</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>2021</v>
@@ -852,13 +1574,13 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G13">
         <v>2021</v>
@@ -866,19 +1588,19 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>21840000</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G14">
         <v>2021</v>
@@ -886,19 +1608,19 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>21840000</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G15">
         <v>2021</v>
@@ -906,19 +1628,19 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>4080</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>2022</v>
@@ -926,19 +1648,19 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>4080</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <v>2022</v>
@@ -949,13 +1671,13 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2022</v>
@@ -966,13 +1688,13 @@
         <v>2022</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G19">
         <v>2022</v>
@@ -983,13 +1705,13 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G20">
         <v>2022</v>
@@ -997,19 +1719,19 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>10920</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G21">
         <v>2022</v>
@@ -1017,19 +1739,19 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C22">
         <v>10920</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G22">
         <v>2022</v>
@@ -1037,19 +1759,19 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>4080</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G23">
         <v>2021</v>
@@ -1057,19 +1779,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>4080</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G24">
         <v>2021</v>
@@ -1080,13 +1802,13 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G25">
         <v>2021</v>
@@ -1097,13 +1819,13 @@
         <v>2021</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G26">
         <v>2021</v>
@@ -1114,13 +1836,13 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G27">
         <v>2021</v>
@@ -1128,19 +1850,19 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>10920</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>2021</v>
@@ -1148,19 +1870,19 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>10920</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G29">
         <v>2021</v>
@@ -1193,30 +1915,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>15000</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>2022</v>
@@ -1224,19 +1946,19 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>15000</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G3">
         <v>2022</v>
@@ -1244,19 +1966,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>15000</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>2021</v>
@@ -1264,19 +1986,19 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>15000</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>2021</v>
@@ -1309,21 +2031,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>121.6</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -1334,13 +2056,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>36491000</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>2022</v>
@@ -1351,16 +2073,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>10.1</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>2021</v>
@@ -1368,16 +2090,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>3029500</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>2021</v>

</xml_diff>